<commit_message>
version 3: stable version
version 3: stable version
</commit_message>
<xml_diff>
--- a/benckmark.xlsx
+++ b/benckmark.xlsx
@@ -649,7 +649,7 @@
     <t>usage</t>
   </si>
   <si>
-    <t>usage/1MB</t>
+    <t>Usage per number of tweets</t>
   </si>
 </sst>
 </file>
@@ -1530,11 +1530,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="307214184"/>
-        <c:axId val="307214576"/>
+        <c:axId val="495675648"/>
+        <c:axId val="495676040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="307214184"/>
+        <c:axId val="495675648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1591,12 +1591,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="307214576"/>
+        <c:crossAx val="495676040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="307214576"/>
+        <c:axId val="495676040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1653,7 +1653,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="307214184"/>
+        <c:crossAx val="495675648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1737,7 +1737,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Performance Graph</a:t>
+              <a:t>Performance per # of tweets</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2546,11 +2546,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="305248968"/>
-        <c:axId val="305249360"/>
+        <c:axId val="495676824"/>
+        <c:axId val="495677216"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="305248968"/>
+        <c:axId val="495676824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2668,12 +2668,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="305249360"/>
+        <c:crossAx val="495677216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="305249360"/>
+        <c:axId val="495677216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2786,7 +2786,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="305248968"/>
+        <c:crossAx val="495676824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2895,7 +2895,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>usage/1MB</c:v>
+                  <c:v>Usage per number of tweets</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3457,16 +3457,72 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="416670752"/>
-        <c:axId val="416669968"/>
+        <c:axId val="494963656"/>
+        <c:axId val="494964048"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="416670752"/>
+        <c:axId val="494963656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t># tweets</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3504,7 +3560,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="416669968"/>
+        <c:crossAx val="494964048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3512,7 +3568,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="416669968"/>
+        <c:axId val="494964048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3532,6 +3588,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>usage (MB)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3563,7 +3675,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="416670752"/>
+        <c:crossAx val="494963656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5679,8 +5791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7332,7 +7444,7 @@
   <dimension ref="A1:E87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>